<commit_message>
Formatted demographics table, put together short descriptives report before class.
</commit_message>
<xml_diff>
--- a/Project0/Processed/DemographicsTable_formatted.xlsx
+++ b/Project0/Processed/DemographicsTable_formatted.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="DemographicsTable" sheetId="1" r:id="rId1"/>
@@ -247,7 +247,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,20 +383,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -574,6 +580,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -766,23 +778,36 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1104,335 +1129,411 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection sqref="A1:F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6"/>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="12" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="10" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="12" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="7" t="s">
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="10" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="10" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="12" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="7" t="s">
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="10" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="7" t="s">
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="12" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="7" t="s">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="10" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="7" t="s">
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="12" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="7" t="s">
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="10" t="s">
         <v>73</v>
       </c>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>